<commit_message>
Fix in "OnlyMuons" column
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2024_v1_0_0/PrescaleTable/L1Menu_Collisions2024_v1_0_0.xlsx
+++ b/development/L1Menu_Collisions2024_v1_0_0/PrescaleTable/L1Menu_Collisions2024_v1_0_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2024_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A66A30-92F9-4448-BB4E-EB928F885291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE3F08F-E9C1-EA48-8A48-C958FED67F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="-19560" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10180" yWindow="-19560" windowWidth="30400" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1262,6 +1262,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1629,7 +1630,7 @@
   <dimension ref="A1:M396"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection sqref="A1:M396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6146,8 +6147,8 @@
       <c r="J110">
         <v>1</v>
       </c>
-      <c r="K110">
-        <v>1</v>
+      <c r="K110" s="1">
+        <v>0</v>
       </c>
       <c r="L110">
         <v>1</v>
@@ -6187,8 +6188,8 @@
       <c r="J111">
         <v>1</v>
       </c>
-      <c r="K111">
-        <v>1</v>
+      <c r="K111" s="1">
+        <v>0</v>
       </c>
       <c r="L111">
         <v>1</v>
@@ -6228,8 +6229,8 @@
       <c r="J112">
         <v>1</v>
       </c>
-      <c r="K112">
-        <v>1</v>
+      <c r="K112" s="1">
+        <v>0</v>
       </c>
       <c r="L112">
         <v>1</v>
@@ -6310,8 +6311,8 @@
       <c r="J114">
         <v>1</v>
       </c>
-      <c r="K114">
-        <v>1</v>
+      <c r="K114" s="1">
+        <v>0</v>
       </c>
       <c r="L114">
         <v>1</v>
@@ -6351,8 +6352,8 @@
       <c r="J115">
         <v>1</v>
       </c>
-      <c r="K115">
-        <v>1</v>
+      <c r="K115" s="1">
+        <v>0</v>
       </c>
       <c r="L115">
         <v>1</v>
@@ -6433,8 +6434,8 @@
       <c r="J117">
         <v>1</v>
       </c>
-      <c r="K117">
-        <v>1</v>
+      <c r="K117" s="1">
+        <v>0</v>
       </c>
       <c r="L117">
         <v>1</v>
@@ -6474,8 +6475,8 @@
       <c r="J118">
         <v>1</v>
       </c>
-      <c r="K118">
-        <v>1</v>
+      <c r="K118" s="1">
+        <v>0</v>
       </c>
       <c r="L118">
         <v>1</v>
@@ -6515,8 +6516,8 @@
       <c r="J119">
         <v>1</v>
       </c>
-      <c r="K119">
-        <v>1</v>
+      <c r="K119" s="1">
+        <v>0</v>
       </c>
       <c r="L119">
         <v>1</v>
@@ -6597,8 +6598,8 @@
       <c r="J121">
         <v>1</v>
       </c>
-      <c r="K121">
-        <v>1</v>
+      <c r="K121" s="1">
+        <v>0</v>
       </c>
       <c r="L121">
         <v>1</v>
@@ -6638,8 +6639,8 @@
       <c r="J122">
         <v>1</v>
       </c>
-      <c r="K122">
-        <v>1</v>
+      <c r="K122" s="1">
+        <v>0</v>
       </c>
       <c r="L122">
         <v>1</v>
@@ -6679,8 +6680,8 @@
       <c r="J123">
         <v>1</v>
       </c>
-      <c r="K123">
-        <v>1</v>
+      <c r="K123" s="1">
+        <v>0</v>
       </c>
       <c r="L123">
         <v>1</v>
@@ -6720,8 +6721,8 @@
       <c r="J124">
         <v>11000</v>
       </c>
-      <c r="K124">
-        <v>11000</v>
+      <c r="K124" s="1">
+        <v>0</v>
       </c>
       <c r="L124">
         <v>11000</v>
@@ -6761,8 +6762,8 @@
       <c r="J125">
         <v>400</v>
       </c>
-      <c r="K125">
-        <v>400</v>
+      <c r="K125" s="1">
+        <v>0</v>
       </c>
       <c r="L125">
         <v>400</v>
@@ -6802,8 +6803,8 @@
       <c r="J126">
         <v>400</v>
       </c>
-      <c r="K126">
-        <v>400</v>
+      <c r="K126" s="1">
+        <v>0</v>
       </c>
       <c r="L126">
         <v>400</v>
@@ -6843,8 +6844,8 @@
       <c r="J127">
         <v>256</v>
       </c>
-      <c r="K127">
-        <v>256</v>
+      <c r="K127" s="1">
+        <v>0</v>
       </c>
       <c r="L127">
         <v>256</v>
@@ -6884,8 +6885,8 @@
       <c r="J128">
         <v>52</v>
       </c>
-      <c r="K128">
-        <v>52</v>
+      <c r="K128" s="1">
+        <v>0</v>
       </c>
       <c r="L128">
         <v>52</v>
@@ -6925,8 +6926,8 @@
       <c r="J129">
         <v>52</v>
       </c>
-      <c r="K129">
-        <v>52</v>
+      <c r="K129" s="1">
+        <v>0</v>
       </c>
       <c r="L129">
         <v>52</v>
@@ -6966,8 +6967,8 @@
       <c r="J130">
         <v>13</v>
       </c>
-      <c r="K130">
-        <v>13</v>
+      <c r="K130" s="1">
+        <v>0</v>
       </c>
       <c r="L130">
         <v>13</v>
@@ -7007,8 +7008,8 @@
       <c r="J131">
         <v>3</v>
       </c>
-      <c r="K131">
-        <v>3</v>
+      <c r="K131" s="1">
+        <v>0</v>
       </c>
       <c r="L131">
         <v>3</v>
@@ -7048,8 +7049,8 @@
       <c r="J132">
         <v>3</v>
       </c>
-      <c r="K132">
-        <v>3</v>
+      <c r="K132" s="1">
+        <v>0</v>
       </c>
       <c r="L132">
         <v>3</v>
@@ -7130,8 +7131,8 @@
       <c r="J134">
         <v>1</v>
       </c>
-      <c r="K134">
-        <v>1</v>
+      <c r="K134" s="1">
+        <v>0</v>
       </c>
       <c r="L134">
         <v>1</v>
@@ -7171,8 +7172,8 @@
       <c r="J135">
         <v>1</v>
       </c>
-      <c r="K135">
-        <v>1</v>
+      <c r="K135" s="1">
+        <v>0</v>
       </c>
       <c r="L135">
         <v>1</v>
@@ -7212,8 +7213,8 @@
       <c r="J136">
         <v>1</v>
       </c>
-      <c r="K136">
-        <v>1</v>
+      <c r="K136" s="1">
+        <v>0</v>
       </c>
       <c r="L136">
         <v>1</v>
@@ -7253,8 +7254,8 @@
       <c r="J137">
         <v>1</v>
       </c>
-      <c r="K137">
-        <v>1</v>
+      <c r="K137" s="1">
+        <v>0</v>
       </c>
       <c r="L137">
         <v>1</v>
@@ -7295,7 +7296,7 @@
         <v>1</v>
       </c>
       <c r="K138" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L138" s="1">
         <v>1</v>
@@ -7336,7 +7337,7 @@
         <v>1</v>
       </c>
       <c r="K139" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L139" s="1">
         <v>1</v>
@@ -7417,8 +7418,8 @@
       <c r="J141">
         <v>1</v>
       </c>
-      <c r="K141">
-        <v>1</v>
+      <c r="K141" s="1">
+        <v>0</v>
       </c>
       <c r="L141">
         <v>1</v>
@@ -7458,8 +7459,8 @@
       <c r="J142">
         <v>1</v>
       </c>
-      <c r="K142">
-        <v>1</v>
+      <c r="K142" s="1">
+        <v>0</v>
       </c>
       <c r="L142">
         <v>1</v>
@@ -7499,8 +7500,8 @@
       <c r="J143">
         <v>1</v>
       </c>
-      <c r="K143">
-        <v>1</v>
+      <c r="K143" s="1">
+        <v>0</v>
       </c>
       <c r="L143">
         <v>1</v>
@@ -7540,8 +7541,8 @@
       <c r="J144">
         <v>1</v>
       </c>
-      <c r="K144">
-        <v>1</v>
+      <c r="K144" s="1">
+        <v>0</v>
       </c>
       <c r="L144">
         <v>1</v>
@@ -7622,8 +7623,8 @@
       <c r="J146">
         <v>1</v>
       </c>
-      <c r="K146">
-        <v>1</v>
+      <c r="K146" s="1">
+        <v>0</v>
       </c>
       <c r="L146">
         <v>1</v>
@@ -7663,8 +7664,8 @@
       <c r="J147">
         <v>1</v>
       </c>
-      <c r="K147">
-        <v>1</v>
+      <c r="K147" s="1">
+        <v>0</v>
       </c>
       <c r="L147">
         <v>1</v>
@@ -7745,8 +7746,8 @@
       <c r="J149">
         <v>1</v>
       </c>
-      <c r="K149">
-        <v>1</v>
+      <c r="K149" s="1">
+        <v>0</v>
       </c>
       <c r="L149">
         <v>1</v>
@@ -7786,8 +7787,8 @@
       <c r="J150">
         <v>1</v>
       </c>
-      <c r="K150">
-        <v>1</v>
+      <c r="K150" s="1">
+        <v>0</v>
       </c>
       <c r="L150">
         <v>1</v>
@@ -7827,8 +7828,8 @@
       <c r="J151">
         <v>1</v>
       </c>
-      <c r="K151">
-        <v>1</v>
+      <c r="K151" s="1">
+        <v>0</v>
       </c>
       <c r="L151">
         <v>1</v>
@@ -7868,8 +7869,8 @@
       <c r="J152">
         <v>1</v>
       </c>
-      <c r="K152">
-        <v>1</v>
+      <c r="K152" s="1">
+        <v>0</v>
       </c>
       <c r="L152">
         <v>1</v>
@@ -7909,8 +7910,8 @@
       <c r="J153">
         <v>1</v>
       </c>
-      <c r="K153">
-        <v>1</v>
+      <c r="K153" s="1">
+        <v>0</v>
       </c>
       <c r="L153">
         <v>1</v>
@@ -7950,8 +7951,8 @@
       <c r="J154">
         <v>1</v>
       </c>
-      <c r="K154">
-        <v>1</v>
+      <c r="K154" s="1">
+        <v>0</v>
       </c>
       <c r="L154">
         <v>1</v>
@@ -7991,8 +7992,8 @@
       <c r="J155">
         <v>1</v>
       </c>
-      <c r="K155">
-        <v>1</v>
+      <c r="K155" s="1">
+        <v>0</v>
       </c>
       <c r="L155">
         <v>1</v>
@@ -8032,8 +8033,8 @@
       <c r="J156">
         <v>44000</v>
       </c>
-      <c r="K156">
-        <v>44000</v>
+      <c r="K156" s="1">
+        <v>0</v>
       </c>
       <c r="L156">
         <v>44000</v>
@@ -8073,8 +8074,8 @@
       <c r="J157">
         <v>9000</v>
       </c>
-      <c r="K157">
-        <v>9000</v>
+      <c r="K157" s="1">
+        <v>0</v>
       </c>
       <c r="L157">
         <v>9000</v>
@@ -8114,8 +8115,8 @@
       <c r="J158">
         <v>1550</v>
       </c>
-      <c r="K158">
-        <v>1550</v>
+      <c r="K158" s="1">
+        <v>0</v>
       </c>
       <c r="L158">
         <v>1550</v>
@@ -8155,8 +8156,8 @@
       <c r="J159">
         <v>780</v>
       </c>
-      <c r="K159">
-        <v>780</v>
+      <c r="K159" s="1">
+        <v>0</v>
       </c>
       <c r="L159">
         <v>780</v>
@@ -8196,8 +8197,8 @@
       <c r="J160">
         <v>45</v>
       </c>
-      <c r="K160">
-        <v>45</v>
+      <c r="K160" s="1">
+        <v>0</v>
       </c>
       <c r="L160">
         <v>45</v>
@@ -8401,8 +8402,8 @@
       <c r="J165">
         <v>1</v>
       </c>
-      <c r="K165">
-        <v>1</v>
+      <c r="K165" s="1">
+        <v>0</v>
       </c>
       <c r="L165">
         <v>1</v>
@@ -8442,8 +8443,8 @@
       <c r="J166">
         <v>1</v>
       </c>
-      <c r="K166">
-        <v>1</v>
+      <c r="K166" s="1">
+        <v>0</v>
       </c>
       <c r="L166">
         <v>1</v>
@@ -8483,8 +8484,8 @@
       <c r="J167">
         <v>1</v>
       </c>
-      <c r="K167">
-        <v>1</v>
+      <c r="K167" s="1">
+        <v>0</v>
       </c>
       <c r="L167">
         <v>1</v>
@@ -8524,8 +8525,8 @@
       <c r="J168">
         <v>1</v>
       </c>
-      <c r="K168">
-        <v>1</v>
+      <c r="K168" s="1">
+        <v>0</v>
       </c>
       <c r="L168">
         <v>1</v>
@@ -8565,8 +8566,8 @@
       <c r="J169">
         <v>1</v>
       </c>
-      <c r="K169">
-        <v>1</v>
+      <c r="K169" s="1">
+        <v>0</v>
       </c>
       <c r="L169">
         <v>1</v>
@@ -8647,8 +8648,8 @@
       <c r="J171">
         <v>1</v>
       </c>
-      <c r="K171">
-        <v>1</v>
+      <c r="K171" s="1">
+        <v>0</v>
       </c>
       <c r="L171">
         <v>1</v>
@@ -9262,8 +9263,8 @@
       <c r="J186">
         <v>25</v>
       </c>
-      <c r="K186">
-        <v>25</v>
+      <c r="K186" s="1">
+        <v>0</v>
       </c>
       <c r="L186">
         <v>25</v>
@@ -9303,8 +9304,8 @@
       <c r="J187">
         <v>1</v>
       </c>
-      <c r="K187">
-        <v>1</v>
+      <c r="K187" s="1">
+        <v>0</v>
       </c>
       <c r="L187">
         <v>1</v>
@@ -9344,8 +9345,8 @@
       <c r="J188">
         <v>1</v>
       </c>
-      <c r="K188">
-        <v>1</v>
+      <c r="K188" s="1">
+        <v>0</v>
       </c>
       <c r="L188">
         <v>1</v>
@@ -9385,8 +9386,8 @@
       <c r="J189">
         <v>1</v>
       </c>
-      <c r="K189">
-        <v>1</v>
+      <c r="K189" s="1">
+        <v>0</v>
       </c>
       <c r="L189">
         <v>1</v>
@@ -9426,8 +9427,8 @@
       <c r="J190">
         <v>1</v>
       </c>
-      <c r="K190">
-        <v>1</v>
+      <c r="K190" s="1">
+        <v>0</v>
       </c>
       <c r="L190">
         <v>1</v>
@@ -9467,8 +9468,8 @@
       <c r="J191">
         <v>1</v>
       </c>
-      <c r="K191">
-        <v>1</v>
+      <c r="K191" s="1">
+        <v>0</v>
       </c>
       <c r="L191">
         <v>1</v>
@@ -9550,7 +9551,7 @@
         <v>2</v>
       </c>
       <c r="K193" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L193" s="1">
         <v>2</v>
@@ -9713,8 +9714,8 @@
       <c r="J197">
         <v>1</v>
       </c>
-      <c r="K197">
-        <v>1</v>
+      <c r="K197" s="1">
+        <v>0</v>
       </c>
       <c r="L197">
         <v>1</v>
@@ -9754,8 +9755,8 @@
       <c r="J198">
         <v>1</v>
       </c>
-      <c r="K198">
-        <v>1</v>
+      <c r="K198" s="1">
+        <v>0</v>
       </c>
       <c r="L198">
         <v>1</v>
@@ -9795,8 +9796,8 @@
       <c r="J199">
         <v>1</v>
       </c>
-      <c r="K199">
-        <v>1</v>
+      <c r="K199" s="1">
+        <v>0</v>
       </c>
       <c r="L199">
         <v>1</v>
@@ -9836,8 +9837,8 @@
       <c r="J200">
         <v>1</v>
       </c>
-      <c r="K200">
-        <v>1</v>
+      <c r="K200" s="1">
+        <v>0</v>
       </c>
       <c r="L200">
         <v>1</v>
@@ -9877,8 +9878,8 @@
       <c r="J201">
         <v>1</v>
       </c>
-      <c r="K201">
-        <v>1</v>
+      <c r="K201" s="1">
+        <v>0</v>
       </c>
       <c r="L201">
         <v>1</v>
@@ -9959,8 +9960,8 @@
       <c r="J203">
         <v>1</v>
       </c>
-      <c r="K203">
-        <v>1</v>
+      <c r="K203" s="1">
+        <v>0</v>
       </c>
       <c r="L203">
         <v>1</v>
@@ -10000,8 +10001,8 @@
       <c r="J204">
         <v>1</v>
       </c>
-      <c r="K204">
-        <v>1</v>
+      <c r="K204" s="1">
+        <v>0</v>
       </c>
       <c r="L204">
         <v>1</v>
@@ -10041,8 +10042,8 @@
       <c r="J205">
         <v>1</v>
       </c>
-      <c r="K205">
-        <v>1</v>
+      <c r="K205" s="1">
+        <v>0</v>
       </c>
       <c r="L205">
         <v>1</v>
@@ -10082,8 +10083,8 @@
       <c r="J206">
         <v>1</v>
       </c>
-      <c r="K206">
-        <v>1</v>
+      <c r="K206" s="1">
+        <v>0</v>
       </c>
       <c r="L206">
         <v>1</v>
@@ -10123,8 +10124,8 @@
       <c r="J207">
         <v>1</v>
       </c>
-      <c r="K207">
-        <v>1</v>
+      <c r="K207" s="1">
+        <v>0</v>
       </c>
       <c r="L207">
         <v>1</v>
@@ -10164,8 +10165,8 @@
       <c r="J208">
         <v>1</v>
       </c>
-      <c r="K208">
-        <v>1</v>
+      <c r="K208" s="1">
+        <v>0</v>
       </c>
       <c r="L208">
         <v>1</v>
@@ -10205,8 +10206,8 @@
       <c r="J209">
         <v>1</v>
       </c>
-      <c r="K209">
-        <v>1</v>
+      <c r="K209" s="1">
+        <v>0</v>
       </c>
       <c r="L209">
         <v>1</v>
@@ -10246,8 +10247,8 @@
       <c r="J210">
         <v>1</v>
       </c>
-      <c r="K210">
-        <v>1</v>
+      <c r="K210" s="1">
+        <v>0</v>
       </c>
       <c r="L210">
         <v>1</v>
@@ -10287,8 +10288,8 @@
       <c r="J211">
         <v>1</v>
       </c>
-      <c r="K211">
-        <v>1</v>
+      <c r="K211" s="1">
+        <v>0</v>
       </c>
       <c r="L211">
         <v>1</v>
@@ -10369,8 +10370,8 @@
       <c r="J213">
         <v>1</v>
       </c>
-      <c r="K213">
-        <v>1</v>
+      <c r="K213" s="1">
+        <v>0</v>
       </c>
       <c r="L213">
         <v>1</v>
@@ -10410,8 +10411,8 @@
       <c r="J214">
         <v>1</v>
       </c>
-      <c r="K214">
-        <v>1</v>
+      <c r="K214" s="1">
+        <v>0</v>
       </c>
       <c r="L214">
         <v>1</v>
@@ -10452,7 +10453,7 @@
         <v>1</v>
       </c>
       <c r="K215" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L215" s="1">
         <v>1</v>
@@ -10493,7 +10494,7 @@
         <v>1</v>
       </c>
       <c r="K216" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L216" s="1">
         <v>1</v>
@@ -10615,8 +10616,8 @@
       <c r="J219">
         <v>1</v>
       </c>
-      <c r="K219">
-        <v>1</v>
+      <c r="K219" s="1">
+        <v>0</v>
       </c>
       <c r="L219">
         <v>1</v>
@@ -10656,8 +10657,8 @@
       <c r="J220">
         <v>1</v>
       </c>
-      <c r="K220">
-        <v>1</v>
+      <c r="K220" s="1">
+        <v>0</v>
       </c>
       <c r="L220">
         <v>1</v>
@@ -10738,8 +10739,8 @@
       <c r="J222">
         <v>1</v>
       </c>
-      <c r="K222">
-        <v>1</v>
+      <c r="K222" s="1">
+        <v>0</v>
       </c>
       <c r="L222">
         <v>1</v>
@@ -10779,8 +10780,8 @@
       <c r="J223">
         <v>1</v>
       </c>
-      <c r="K223">
-        <v>1</v>
+      <c r="K223" s="1">
+        <v>0</v>
       </c>
       <c r="L223">
         <v>1</v>
@@ -10820,8 +10821,8 @@
       <c r="J224">
         <v>1</v>
       </c>
-      <c r="K224">
-        <v>1</v>
+      <c r="K224" s="1">
+        <v>0</v>
       </c>
       <c r="L224">
         <v>1</v>
@@ -10861,8 +10862,8 @@
       <c r="J225">
         <v>1</v>
       </c>
-      <c r="K225">
-        <v>1</v>
+      <c r="K225" s="1">
+        <v>0</v>
       </c>
       <c r="L225">
         <v>1</v>
@@ -10902,8 +10903,8 @@
       <c r="J226">
         <v>1</v>
       </c>
-      <c r="K226">
-        <v>1</v>
+      <c r="K226" s="1">
+        <v>0</v>
       </c>
       <c r="L226">
         <v>1</v>
@@ -11025,8 +11026,8 @@
       <c r="J229">
         <v>1</v>
       </c>
-      <c r="K229">
-        <v>1</v>
+      <c r="K229" s="1">
+        <v>0</v>
       </c>
       <c r="L229">
         <v>1</v>
@@ -11066,8 +11067,8 @@
       <c r="J230">
         <v>1</v>
       </c>
-      <c r="K230">
-        <v>1</v>
+      <c r="K230" s="1">
+        <v>0</v>
       </c>
       <c r="L230">
         <v>1</v>
@@ -11107,8 +11108,8 @@
       <c r="J231">
         <v>1</v>
       </c>
-      <c r="K231">
-        <v>1</v>
+      <c r="K231" s="1">
+        <v>0</v>
       </c>
       <c r="L231">
         <v>1</v>
@@ -11271,8 +11272,8 @@
       <c r="J235">
         <v>1</v>
       </c>
-      <c r="K235">
-        <v>1</v>
+      <c r="K235" s="1">
+        <v>0</v>
       </c>
       <c r="L235">
         <v>1</v>
@@ -11312,8 +11313,8 @@
       <c r="J236">
         <v>1</v>
       </c>
-      <c r="K236">
-        <v>1</v>
+      <c r="K236" s="1">
+        <v>0</v>
       </c>
       <c r="L236">
         <v>1</v>
@@ -11353,8 +11354,8 @@
       <c r="J237">
         <v>1</v>
       </c>
-      <c r="K237">
-        <v>1</v>
+      <c r="K237" s="1">
+        <v>0</v>
       </c>
       <c r="L237">
         <v>1</v>
@@ -11435,8 +11436,8 @@
       <c r="J239">
         <v>1</v>
       </c>
-      <c r="K239">
-        <v>1</v>
+      <c r="K239" s="1">
+        <v>0</v>
       </c>
       <c r="L239">
         <v>1</v>
@@ -11476,8 +11477,8 @@
       <c r="J240">
         <v>1</v>
       </c>
-      <c r="K240">
-        <v>1</v>
+      <c r="K240" s="1">
+        <v>0</v>
       </c>
       <c r="L240">
         <v>1</v>
@@ -11517,8 +11518,8 @@
       <c r="J241">
         <v>1</v>
       </c>
-      <c r="K241">
-        <v>1</v>
+      <c r="K241" s="1">
+        <v>0</v>
       </c>
       <c r="L241">
         <v>1</v>
@@ -11558,8 +11559,8 @@
       <c r="J242">
         <v>1</v>
       </c>
-      <c r="K242">
-        <v>1</v>
+      <c r="K242" s="1">
+        <v>0</v>
       </c>
       <c r="L242">
         <v>1</v>
@@ -11599,8 +11600,8 @@
       <c r="J243">
         <v>1</v>
       </c>
-      <c r="K243">
-        <v>1</v>
+      <c r="K243" s="1">
+        <v>0</v>
       </c>
       <c r="L243">
         <v>1</v>
@@ -11640,8 +11641,8 @@
       <c r="J244">
         <v>1</v>
       </c>
-      <c r="K244">
-        <v>1</v>
+      <c r="K244" s="1">
+        <v>0</v>
       </c>
       <c r="L244">
         <v>1</v>
@@ -11722,8 +11723,8 @@
       <c r="J246">
         <v>1</v>
       </c>
-      <c r="K246">
-        <v>1</v>
+      <c r="K246" s="1">
+        <v>0</v>
       </c>
       <c r="L246">
         <v>1</v>
@@ -11763,8 +11764,8 @@
       <c r="J247">
         <v>1</v>
       </c>
-      <c r="K247">
-        <v>1</v>
+      <c r="K247" s="1">
+        <v>0</v>
       </c>
       <c r="L247">
         <v>1</v>
@@ -11804,8 +11805,8 @@
       <c r="J248">
         <v>1</v>
       </c>
-      <c r="K248">
-        <v>1</v>
+      <c r="K248" s="1">
+        <v>0</v>
       </c>
       <c r="L248">
         <v>1</v>
@@ -11845,8 +11846,8 @@
       <c r="J249">
         <v>1</v>
       </c>
-      <c r="K249">
-        <v>1</v>
+      <c r="K249" s="1">
+        <v>0</v>
       </c>
       <c r="L249">
         <v>1</v>
@@ -11886,8 +11887,8 @@
       <c r="J250">
         <v>190</v>
       </c>
-      <c r="K250">
-        <v>190</v>
+      <c r="K250" s="1">
+        <v>0</v>
       </c>
       <c r="L250">
         <v>190</v>
@@ -11927,8 +11928,8 @@
       <c r="J251">
         <v>64000</v>
       </c>
-      <c r="K251">
-        <v>64000</v>
+      <c r="K251" s="1">
+        <v>0</v>
       </c>
       <c r="L251">
         <v>64000</v>
@@ -11968,8 +11969,8 @@
       <c r="J252">
         <v>17000</v>
       </c>
-      <c r="K252">
-        <v>17000</v>
+      <c r="K252" s="1">
+        <v>0</v>
       </c>
       <c r="L252">
         <v>17000</v>
@@ -12009,8 +12010,8 @@
       <c r="J253">
         <v>1500</v>
       </c>
-      <c r="K253">
-        <v>1500</v>
+      <c r="K253" s="1">
+        <v>0</v>
       </c>
       <c r="L253">
         <v>1500</v>
@@ -12050,8 +12051,8 @@
       <c r="J254">
         <v>350</v>
       </c>
-      <c r="K254">
-        <v>350</v>
+      <c r="K254" s="1">
+        <v>0</v>
       </c>
       <c r="L254">
         <v>350</v>
@@ -12091,8 +12092,8 @@
       <c r="J255">
         <v>1</v>
       </c>
-      <c r="K255">
-        <v>1</v>
+      <c r="K255" s="1">
+        <v>0</v>
       </c>
       <c r="L255">
         <v>1</v>
@@ -12132,8 +12133,8 @@
       <c r="J256">
         <v>1</v>
       </c>
-      <c r="K256">
-        <v>1</v>
+      <c r="K256" s="1">
+        <v>0</v>
       </c>
       <c r="L256">
         <v>1</v>
@@ -12419,8 +12420,8 @@
       <c r="J263">
         <v>1</v>
       </c>
-      <c r="K263">
-        <v>1</v>
+      <c r="K263" s="1">
+        <v>0</v>
       </c>
       <c r="L263">
         <v>1</v>
@@ -12460,8 +12461,8 @@
       <c r="J264">
         <v>28327</v>
       </c>
-      <c r="K264">
-        <v>28327</v>
+      <c r="K264" s="1">
+        <v>0</v>
       </c>
       <c r="L264">
         <v>28327</v>
@@ -12501,8 +12502,8 @@
       <c r="J265">
         <v>1820</v>
       </c>
-      <c r="K265">
-        <v>1820</v>
+      <c r="K265" s="1">
+        <v>0</v>
       </c>
       <c r="L265">
         <v>1820</v>
@@ -12542,8 +12543,8 @@
       <c r="J266">
         <v>264</v>
       </c>
-      <c r="K266">
-        <v>264</v>
+      <c r="K266" s="1">
+        <v>0</v>
       </c>
       <c r="L266">
         <v>264</v>
@@ -12583,8 +12584,8 @@
       <c r="J267">
         <v>45</v>
       </c>
-      <c r="K267">
-        <v>45</v>
+      <c r="K267" s="1">
+        <v>0</v>
       </c>
       <c r="L267">
         <v>45</v>
@@ -12952,8 +12953,8 @@
       <c r="J276">
         <v>1</v>
       </c>
-      <c r="K276">
-        <v>1</v>
+      <c r="K276" s="1">
+        <v>0</v>
       </c>
       <c r="L276">
         <v>1</v>
@@ -12993,8 +12994,8 @@
       <c r="J277">
         <v>1</v>
       </c>
-      <c r="K277">
-        <v>1</v>
+      <c r="K277" s="1">
+        <v>0</v>
       </c>
       <c r="L277">
         <v>1</v>
@@ -13034,8 +13035,8 @@
       <c r="J278">
         <v>1</v>
       </c>
-      <c r="K278">
-        <v>1</v>
+      <c r="K278" s="1">
+        <v>0</v>
       </c>
       <c r="L278">
         <v>1</v>
@@ -13075,8 +13076,8 @@
       <c r="J279">
         <v>1</v>
       </c>
-      <c r="K279">
-        <v>1</v>
+      <c r="K279" s="1">
+        <v>0</v>
       </c>
       <c r="L279">
         <v>1</v>
@@ -13116,8 +13117,8 @@
       <c r="J280">
         <v>8400</v>
       </c>
-      <c r="K280">
-        <v>8400</v>
+      <c r="K280" s="1">
+        <v>0</v>
       </c>
       <c r="L280">
         <v>8400</v>
@@ -13157,8 +13158,8 @@
       <c r="J281">
         <v>170</v>
       </c>
-      <c r="K281">
-        <v>170</v>
+      <c r="K281" s="1">
+        <v>0</v>
       </c>
       <c r="L281">
         <v>170</v>
@@ -13198,8 +13199,8 @@
       <c r="J282">
         <v>70</v>
       </c>
-      <c r="K282">
-        <v>70</v>
+      <c r="K282" s="1">
+        <v>0</v>
       </c>
       <c r="L282">
         <v>70</v>
@@ -13239,8 +13240,8 @@
       <c r="J283">
         <v>1</v>
       </c>
-      <c r="K283">
-        <v>1</v>
+      <c r="K283" s="1">
+        <v>0</v>
       </c>
       <c r="L283">
         <v>1</v>
@@ -13321,8 +13322,8 @@
       <c r="J285">
         <v>1</v>
       </c>
-      <c r="K285">
-        <v>1</v>
+      <c r="K285" s="1">
+        <v>0</v>
       </c>
       <c r="L285">
         <v>1</v>
@@ -13403,8 +13404,8 @@
       <c r="J287">
         <v>1</v>
       </c>
-      <c r="K287">
-        <v>1</v>
+      <c r="K287" s="1">
+        <v>0</v>
       </c>
       <c r="L287">
         <v>1</v>
@@ -13444,8 +13445,8 @@
       <c r="J288">
         <v>1</v>
       </c>
-      <c r="K288">
-        <v>1</v>
+      <c r="K288" s="1">
+        <v>0</v>
       </c>
       <c r="L288">
         <v>1</v>
@@ -13485,8 +13486,8 @@
       <c r="J289">
         <v>1</v>
       </c>
-      <c r="K289">
-        <v>1</v>
+      <c r="K289" s="1">
+        <v>0</v>
       </c>
       <c r="L289">
         <v>1</v>
@@ -13526,8 +13527,8 @@
       <c r="J290">
         <v>1</v>
       </c>
-      <c r="K290">
-        <v>1</v>
+      <c r="K290" s="1">
+        <v>0</v>
       </c>
       <c r="L290">
         <v>1</v>
@@ -13568,7 +13569,7 @@
         <v>1</v>
       </c>
       <c r="K291" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L291" s="1">
         <v>1</v>
@@ -13609,7 +13610,7 @@
         <v>1</v>
       </c>
       <c r="K292" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L292" s="1">
         <v>1</v>
@@ -13650,7 +13651,7 @@
         <v>1</v>
       </c>
       <c r="K293" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L293" s="1">
         <v>1</v>
@@ -13691,7 +13692,7 @@
         <v>1</v>
       </c>
       <c r="K294" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L294" s="1">
         <v>1</v>
@@ -13732,7 +13733,7 @@
         <v>1</v>
       </c>
       <c r="K295" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L295" s="1">
         <v>1</v>
@@ -13773,7 +13774,7 @@
         <v>1</v>
       </c>
       <c r="K296" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L296" s="1">
         <v>1</v>
@@ -13814,7 +13815,7 @@
         <v>1</v>
       </c>
       <c r="K297" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L297" s="1">
         <v>1</v>
@@ -13855,7 +13856,7 @@
         <v>1</v>
       </c>
       <c r="K298" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L298" s="1">
         <v>1</v>
@@ -13896,7 +13897,7 @@
         <v>1</v>
       </c>
       <c r="K299" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L299" s="1">
         <v>1</v>
@@ -13937,7 +13938,7 @@
         <v>1</v>
       </c>
       <c r="K300" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L300" s="1">
         <v>1</v>
@@ -13978,7 +13979,7 @@
         <v>1</v>
       </c>
       <c r="K301" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L301" s="1">
         <v>1</v>
@@ -14018,8 +14019,8 @@
       <c r="J302">
         <v>1</v>
       </c>
-      <c r="K302">
-        <v>1</v>
+      <c r="K302" s="1">
+        <v>0</v>
       </c>
       <c r="L302">
         <v>1</v>
@@ -14059,8 +14060,8 @@
       <c r="J303">
         <v>1</v>
       </c>
-      <c r="K303">
-        <v>1</v>
+      <c r="K303" s="1">
+        <v>0</v>
       </c>
       <c r="L303">
         <v>1</v>
@@ -14100,8 +14101,8 @@
       <c r="J304">
         <v>1</v>
       </c>
-      <c r="K304">
-        <v>1</v>
+      <c r="K304" s="1">
+        <v>0</v>
       </c>
       <c r="L304">
         <v>1</v>
@@ -14141,8 +14142,8 @@
       <c r="J305">
         <v>1</v>
       </c>
-      <c r="K305">
-        <v>1</v>
+      <c r="K305" s="1">
+        <v>0</v>
       </c>
       <c r="L305">
         <v>1</v>
@@ -14223,8 +14224,8 @@
       <c r="J307">
         <v>1</v>
       </c>
-      <c r="K307">
-        <v>1</v>
+      <c r="K307" s="1">
+        <v>0</v>
       </c>
       <c r="L307">
         <v>1</v>
@@ -14264,8 +14265,8 @@
       <c r="J308">
         <v>100</v>
       </c>
-      <c r="K308">
-        <v>100</v>
+      <c r="K308" s="1">
+        <v>0</v>
       </c>
       <c r="L308">
         <v>100</v>
@@ -14305,8 +14306,8 @@
       <c r="J309">
         <v>50</v>
       </c>
-      <c r="K309">
-        <v>50</v>
+      <c r="K309" s="1">
+        <v>0</v>
       </c>
       <c r="L309">
         <v>50</v>
@@ -14346,8 +14347,8 @@
       <c r="J310">
         <v>1</v>
       </c>
-      <c r="K310">
-        <v>1</v>
+      <c r="K310" s="1">
+        <v>0</v>
       </c>
       <c r="L310">
         <v>1</v>
@@ -14387,8 +14388,8 @@
       <c r="J311">
         <v>1</v>
       </c>
-      <c r="K311">
-        <v>1</v>
+      <c r="K311" s="1">
+        <v>0</v>
       </c>
       <c r="L311">
         <v>1</v>
@@ -14428,8 +14429,8 @@
       <c r="J312">
         <v>1</v>
       </c>
-      <c r="K312">
-        <v>1</v>
+      <c r="K312" s="1">
+        <v>0</v>
       </c>
       <c r="L312">
         <v>1</v>
@@ -14469,8 +14470,8 @@
       <c r="J313">
         <v>1</v>
       </c>
-      <c r="K313">
-        <v>1</v>
+      <c r="K313" s="1">
+        <v>0</v>
       </c>
       <c r="L313">
         <v>1</v>
@@ -14510,8 +14511,8 @@
       <c r="J314">
         <v>1</v>
       </c>
-      <c r="K314">
-        <v>1</v>
+      <c r="K314" s="1">
+        <v>0</v>
       </c>
       <c r="L314">
         <v>1</v>
@@ -14551,8 +14552,8 @@
       <c r="J315">
         <v>1</v>
       </c>
-      <c r="K315">
-        <v>1</v>
+      <c r="K315" s="1">
+        <v>0</v>
       </c>
       <c r="L315">
         <v>1</v>
@@ -14592,8 +14593,8 @@
       <c r="J316">
         <v>11400</v>
       </c>
-      <c r="K316">
-        <v>11400</v>
+      <c r="K316" s="1">
+        <v>0</v>
       </c>
       <c r="L316">
         <v>11400</v>
@@ -14633,8 +14634,8 @@
       <c r="J317">
         <v>4100</v>
       </c>
-      <c r="K317">
-        <v>4100</v>
+      <c r="K317" s="1">
+        <v>0</v>
       </c>
       <c r="L317">
         <v>4100</v>
@@ -14674,8 +14675,8 @@
       <c r="J318">
         <v>1600</v>
       </c>
-      <c r="K318">
-        <v>1600</v>
+      <c r="K318" s="1">
+        <v>0</v>
       </c>
       <c r="L318">
         <v>1600</v>
@@ -14715,8 +14716,8 @@
       <c r="J319">
         <v>500</v>
       </c>
-      <c r="K319">
-        <v>500</v>
+      <c r="K319" s="1">
+        <v>0</v>
       </c>
       <c r="L319">
         <v>500</v>
@@ -14756,8 +14757,8 @@
       <c r="J320">
         <v>1</v>
       </c>
-      <c r="K320">
-        <v>1</v>
+      <c r="K320" s="1">
+        <v>0</v>
       </c>
       <c r="L320">
         <v>1</v>
@@ -14797,8 +14798,8 @@
       <c r="J321">
         <v>1</v>
       </c>
-      <c r="K321">
-        <v>1</v>
+      <c r="K321" s="1">
+        <v>0</v>
       </c>
       <c r="L321">
         <v>1</v>
@@ -14838,8 +14839,8 @@
       <c r="J322">
         <v>1</v>
       </c>
-      <c r="K322">
-        <v>1</v>
+      <c r="K322" s="1">
+        <v>0</v>
       </c>
       <c r="L322">
         <v>1</v>
@@ -14879,8 +14880,8 @@
       <c r="J323">
         <v>1</v>
       </c>
-      <c r="K323">
-        <v>1</v>
+      <c r="K323" s="1">
+        <v>0</v>
       </c>
       <c r="L323">
         <v>1</v>
@@ -14920,8 +14921,8 @@
       <c r="J324">
         <v>1</v>
       </c>
-      <c r="K324">
-        <v>1</v>
+      <c r="K324" s="1">
+        <v>0</v>
       </c>
       <c r="L324">
         <v>1</v>
@@ -15002,8 +15003,8 @@
       <c r="J326">
         <v>1</v>
       </c>
-      <c r="K326">
-        <v>1</v>
+      <c r="K326" s="1">
+        <v>0</v>
       </c>
       <c r="L326">
         <v>1</v>
@@ -15084,8 +15085,8 @@
       <c r="J328">
         <v>1</v>
       </c>
-      <c r="K328">
-        <v>1</v>
+      <c r="K328" s="1">
+        <v>0</v>
       </c>
       <c r="L328">
         <v>1</v>
@@ -15207,8 +15208,8 @@
       <c r="J331">
         <v>1</v>
       </c>
-      <c r="K331">
-        <v>1</v>
+      <c r="K331" s="1">
+        <v>0</v>
       </c>
       <c r="L331">
         <v>1</v>
@@ -15248,8 +15249,8 @@
       <c r="J332">
         <v>1</v>
       </c>
-      <c r="K332">
-        <v>1</v>
+      <c r="K332" s="1">
+        <v>0</v>
       </c>
       <c r="L332">
         <v>1</v>
@@ -15289,8 +15290,8 @@
       <c r="J333">
         <v>1</v>
       </c>
-      <c r="K333">
-        <v>1</v>
+      <c r="K333" s="1">
+        <v>0</v>
       </c>
       <c r="L333">
         <v>1</v>
@@ -15330,8 +15331,8 @@
       <c r="J334">
         <v>1</v>
       </c>
-      <c r="K334">
-        <v>1</v>
+      <c r="K334" s="1">
+        <v>0</v>
       </c>
       <c r="L334">
         <v>1</v>
@@ -15371,8 +15372,8 @@
       <c r="J335">
         <v>1</v>
       </c>
-      <c r="K335">
-        <v>1</v>
+      <c r="K335" s="1">
+        <v>0</v>
       </c>
       <c r="L335">
         <v>1</v>
@@ -15412,8 +15413,8 @@
       <c r="J336">
         <v>1</v>
       </c>
-      <c r="K336">
-        <v>1</v>
+      <c r="K336" s="1">
+        <v>0</v>
       </c>
       <c r="L336">
         <v>1</v>
@@ -15453,8 +15454,8 @@
       <c r="J337">
         <v>1</v>
       </c>
-      <c r="K337">
-        <v>1</v>
+      <c r="K337" s="1">
+        <v>0</v>
       </c>
       <c r="L337">
         <v>1</v>
@@ -15576,8 +15577,8 @@
       <c r="J340">
         <v>1</v>
       </c>
-      <c r="K340">
-        <v>1</v>
+      <c r="K340" s="1">
+        <v>0</v>
       </c>
       <c r="L340">
         <v>1</v>
@@ -15617,8 +15618,8 @@
       <c r="J341">
         <v>1</v>
       </c>
-      <c r="K341">
-        <v>1</v>
+      <c r="K341" s="1">
+        <v>0</v>
       </c>
       <c r="L341">
         <v>1</v>
@@ -15658,8 +15659,8 @@
       <c r="J342">
         <v>1</v>
       </c>
-      <c r="K342">
-        <v>1</v>
+      <c r="K342" s="1">
+        <v>0</v>
       </c>
       <c r="L342">
         <v>1</v>
@@ -15699,8 +15700,8 @@
       <c r="J343">
         <v>1</v>
       </c>
-      <c r="K343">
-        <v>1</v>
+      <c r="K343" s="1">
+        <v>0</v>
       </c>
       <c r="L343">
         <v>1</v>
@@ -15740,8 +15741,8 @@
       <c r="J344">
         <v>1</v>
       </c>
-      <c r="K344">
-        <v>1</v>
+      <c r="K344" s="1">
+        <v>0</v>
       </c>
       <c r="L344">
         <v>1</v>

</xml_diff>